<commit_message>
Refactor email generation and update report files
Refactored the geracao_email function in 3 - envio_relatorios.py to dynamically load company-specific report files and handle missing files gracefully. Updated and removed several Excel report files, added a new PDF report, and deleted obsolete files to reflect the latest reporting data.
</commit_message>
<xml_diff>
--- a/Integration Quality/EMPRESAS/Relatorio - INOVENTS.xlsx
+++ b/Integration Quality/EMPRESAS/Relatorio - INOVENTS.xlsx
@@ -711,14 +711,14 @@
         </is>
       </c>
       <c r="D2" s="6" t="n">
-        <v>41285.38472222222</v>
+        <v>41285.38523148148</v>
       </c>
       <c r="E2" s="6" t="n">
-        <v>45819.47986111111</v>
+        <v>45826.70905092593</v>
       </c>
       <c r="F2" s="5" t="inlineStr">
         <is>
-          <t>09 a 15 dias</t>
+          <t>06 a 08 dias</t>
         </is>
       </c>
       <c r="G2" s="5" t="inlineStr">

</xml_diff>